<commit_message>
Actualizacion datos generales de la denuncia
</commit_message>
<xml_diff>
--- a/Observaciones a formulario Web Tecmar (Ruth)/Obserbaciones Formulario Prototipo.xlsx
+++ b/Observaciones a formulario Web Tecmar (Ruth)/Obserbaciones Formulario Prototipo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="197">
   <si>
     <t>formularios</t>
   </si>
@@ -540,9 +540,6 @@
     <t>109 observaciones</t>
   </si>
   <si>
-    <t>*** problemática</t>
-  </si>
-  <si>
     <t>x polmar</t>
   </si>
   <si>
@@ -607,6 +604,9 @@
   </si>
   <si>
     <t>Glidentificador , ruth = no estaba en el formulario anterior</t>
+  </si>
+  <si>
+    <t>*** problemática 25</t>
   </si>
 </sst>
 </file>
@@ -947,15 +947,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1020,7 +1020,7 @@
         <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1125,7 +1125,7 @@
         <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1142,13 +1142,13 @@
         <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F13" t="s">
         <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D23" t="s">
         <v>27</v>
@@ -1494,7 +1494,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
@@ -1619,7 +1619,7 @@
         <v>64</v>
       </c>
       <c r="G43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>64</v>
       </c>
       <c r="G44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1676,7 +1676,7 @@
         <v>64</v>
       </c>
       <c r="G46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
         <v>64</v>
       </c>
       <c r="G50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1849,10 +1849,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D56" t="s">
         <v>160</v>
@@ -1895,7 +1895,7 @@
         <v>67</v>
       </c>
       <c r="G59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
         <v>67</v>
       </c>
       <c r="G60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1969,7 +1969,7 @@
         <v>67</v>
       </c>
       <c r="G63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>70</v>
       </c>
       <c r="C79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E79" t="s">
         <v>9</v>
@@ -2261,7 +2261,7 @@
         <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E80" t="s">
         <v>9</v>
@@ -2312,7 +2312,7 @@
         <v>75</v>
       </c>
       <c r="C83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E83" t="s">
         <v>9</v>
@@ -2329,10 +2329,10 @@
         <v>76</v>
       </c>
       <c r="C84" t="s">
+        <v>178</v>
+      </c>
+      <c r="E84" t="s">
         <v>179</v>
-      </c>
-      <c r="E84" t="s">
-        <v>180</v>
       </c>
       <c r="F84" t="s">
         <v>67</v>
@@ -2432,7 +2432,7 @@
         <v>85</v>
       </c>
       <c r="G90" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>160</v>
       </c>
       <c r="E91" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F91" t="s">
         <v>85</v>
@@ -2647,10 +2647,10 @@
         <v>84</v>
       </c>
       <c r="B103" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C103" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D103" t="s">
         <v>160</v>
@@ -2664,7 +2664,7 @@
         <v>84</v>
       </c>
       <c r="B104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C104" t="s">
         <v>138</v>
@@ -2800,13 +2800,13 @@
         <v>104</v>
       </c>
       <c r="C114" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D114" t="s">
         <v>160</v>
       </c>
       <c r="E114" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F114" t="s">
         <v>101</v>
@@ -2820,13 +2820,13 @@
         <v>105</v>
       </c>
       <c r="C115" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D115" t="s">
         <v>160</v>
       </c>
       <c r="E115" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F115" t="s">
         <v>101</v>
@@ -2840,13 +2840,13 @@
         <v>106</v>
       </c>
       <c r="C116" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D116" t="s">
         <v>160</v>
       </c>
       <c r="E116" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F116" t="s">
         <v>101</v>
@@ -2894,13 +2894,16 @@
         <v>109</v>
       </c>
       <c r="C120" t="s">
-        <v>193</v>
+        <v>192</v>
+      </c>
+      <c r="D120" t="s">
+        <v>160</v>
       </c>
       <c r="F120" t="s">
         <v>110</v>
       </c>
       <c r="G120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -2922,15 +2925,15 @@
         <v>173</v>
       </c>
       <c r="C123" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
+        <v>196</v>
+      </c>
+      <c r="C124" t="s">
         <v>174</v>
-      </c>
-      <c r="C124" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>